<commit_message>
Service code changes with mongo
</commit_message>
<xml_diff>
--- a/src/main/resources/static/MTS_Database_Schema.xlsx
+++ b/src/main/resources/static/MTS_Database_Schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\movie-ticket-service\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3429BC22-B730-4B37-A050-01B7828B1774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367608C7-D8C0-40FC-877F-24CC412B9F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{54A43033-A4FC-4481-B143-F3F3B14245E8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>USER_DETAILS</t>
   </si>
@@ -210,11 +210,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -535,7 +536,7 @@
   <dimension ref="D4:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,18 +550,18 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="E4" s="5"/>
+      <c r="G4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="H4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="4"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
@@ -654,18 +655,18 @@
     </row>
     <row r="11" spans="4:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="G12" s="4" t="s">
+      <c r="E12" s="5"/>
+      <c r="G12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="J12" s="4" t="s">
+      <c r="H12" s="5"/>
+      <c r="J12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="4"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
@@ -694,10 +695,10 @@
       <c r="E14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="G14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J14" s="3" t="s">
@@ -715,10 +716,10 @@
         <v>7</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>14</v>
@@ -734,10 +735,10 @@
       <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="G16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -748,17 +749,17 @@
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>34</v>
@@ -773,12 +774,6 @@
       </c>
       <c r="E18" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>35</v>

</xml_diff>